<commit_message>
Date.local_parse for all imports and other places
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_commitments.xlsx
+++ b/public/sample_uploads/capital_commitments.xlsx
@@ -22,8 +22,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>Author</author>
-    <author>thimm</author>
+    <author>Unknown Author</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0">
@@ -95,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="1">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -472,7 +471,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="35">
   <si>
     <t xml:space="preserve">Investor *</t>
   </si>
@@ -544,6 +543,9 @@
   </si>
   <si>
     <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20/01/2023</t>
   </si>
   <si>
     <t xml:space="preserve">signatory1@gmail.com,signatory2@gmail.com</t>
@@ -725,39 +727,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1020,11 +1022,11 @@
   </sheetPr>
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q2" activeCellId="0" sqref="Q2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K2:K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.56"/>
@@ -1130,19 +1132,19 @@
       <c r="I2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="6" t="n">
-        <v>44946</v>
+      <c r="K2" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>19</v>
@@ -1164,21 +1166,21 @@
         <v>22</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="6" t="n">
-        <v>44946</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="R3" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>19</v>
@@ -1194,7 +1196,7 @@
         <v>8</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>22</v>
@@ -1202,19 +1204,19 @@
       <c r="I4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="6" t="n">
-        <v>44946</v>
+      <c r="K4" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>19</v>
@@ -1230,7 +1232,7 @@
         <v>9</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>22</v>
@@ -1238,19 +1240,19 @@
       <c r="I5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="6" t="n">
-        <v>44946</v>
+      <c r="K5" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>19</v>
@@ -1266,7 +1268,7 @@
         <v>10</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>22</v>
@@ -1274,14 +1276,14 @@
       <c r="I6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="6" t="n">
-        <v>44946</v>
+      <c r="K6" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1299,7 +1301,7 @@
         <v>20</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>21</v>
@@ -1310,19 +1312,19 @@
       <c r="I7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="6" t="n">
-        <v>44946</v>
+      <c r="K7" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>19</v>
@@ -1338,7 +1340,7 @@
         <v>11</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>22</v>
@@ -1346,19 +1348,19 @@
       <c r="I8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="6" t="n">
-        <v>44946</v>
+      <c r="K8" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>19</v>
@@ -1374,7 +1376,7 @@
         <v>12</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>22</v>
@@ -1382,14 +1384,14 @@
       <c r="I9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K9" s="6" t="n">
-        <v>44946</v>
+      <c r="K9" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>